<commit_message>
audio dac and udp optimization. m4 not used
</commit_message>
<xml_diff>
--- a/Documentation/filters.xlsx
+++ b/Documentation/filters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_DOCUMENTS\Embedded Systems\EmbeddedSystemsProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFD70750-7338-46E9-9C28-B6B935D7BE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E605FF4-E9C9-48E8-8681-79867B7B5937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29550" yWindow="-2240" windowWidth="29660" windowHeight="17900" activeTab="1" xr2:uid="{B5FAC551-6717-451E-9ECF-BEE48E47EDAE}"/>
+    <workbookView xWindow="-14810" yWindow="-2130" windowWidth="14900" windowHeight="17770" activeTab="1" xr2:uid="{B5FAC551-6717-451E-9ECF-BEE48E47EDAE}"/>
   </bookViews>
   <sheets>
     <sheet name="1st Order Low Pass RC Filter" sheetId="1" r:id="rId1"/>
@@ -308,64 +308,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.31415768346733924</c:v>
+                  <c:v>4.1433053025334177</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62830587817976513</c:v>
+                  <c:v>8.2651418011813451</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2565358503006416</c:v>
+                  <c:v>16.361808227092183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5124647270906517</c:v>
+                  <c:v>31.47199873503833</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0200824462712461</c:v>
+                  <c:v>55.20263830241327</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.001667440278894</c:v>
+                  <c:v>79.606907125061667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.703979870138081</c:v>
+                  <c:v>93.161604998713926</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.256523983928432</c:v>
+                  <c:v>97.764882339801204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.423408165778447</c:v>
+                  <c:v>98.930360325690771</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>84.307069028376134</c:v>
+                  <c:v>98.843449304697174</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94.586936077977313</c:v>
+                  <c:v>97.326914561755274</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.682873915180423</c:v>
+                  <c:v>91.650334636322967</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98.01759388716647</c:v>
+                  <c:v>75.998710268032823</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.215303766608372</c:v>
+                  <c:v>50.668258089959579</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.276980423049977</c:v>
+                  <c:v>28.227190444305368</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>71.490182840868755</c:v>
+                  <c:v>14.55983081775633</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45.807590627916838</c:v>
+                  <c:v>7.3390814730506264</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.99820912271597</c:v>
+                  <c:v>3.6770498794155375</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12.809059052119235</c:v>
+                  <c:v>1.8394671893419614</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.4451089229073135</c:v>
+                  <c:v>0.9198514890924202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,14 +1206,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1251,7 +1247,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1357,7 +1353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1499,7 +1495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1513,12 +1509,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1534,7 +1530,7 @@
         <v>4.6999999999999997E-8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1542,7 +1538,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1550,12 +1546,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1579,7 +1575,7 @@
         <v>9.9999903679097013</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1592,7 +1588,7 @@
         <v>9.9990369287223402</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>100</v>
       </c>
@@ -1605,7 +1601,7 @@
         <v>9.9050486484486626</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" ref="A11:A64" si="2">A10*1.3</f>
         <v>130</v>
@@ -1619,7 +1615,7 @@
         <v>9.8410873116548174</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>169</v>
@@ -1633,7 +1629,7 @@
         <v>9.7357530553361524</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>219.70000000000002</v>
@@ -1647,7 +1643,7 @@
         <v>9.5651760492339939</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>285.61</v>
@@ -1661,7 +1657,7 @@
         <v>9.2962176599375823</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>371.29300000000001</v>
@@ -1675,7 +1671,7 @@
         <v>8.8890698429601791</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>482.68090000000001</v>
@@ -1689,7 +1685,7 @@
         <v>8.307931527140008</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="2"/>
         <v>627.48517000000004</v>
@@ -1703,7 +1699,7 @@
         <v>7.5409883722779538</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="2"/>
         <v>815.73072100000013</v>
@@ -1717,7 +1713,7 @@
         <v>6.6199440647015875</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="2"/>
         <v>1060.4499373000001</v>
@@ -1731,7 +1727,7 @@
         <v>5.6197830887322793</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="2"/>
         <v>1378.5849184900003</v>
@@ -1745,7 +1741,7 @@
         <v>4.631836157752808</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>1792.1603940370005</v>
@@ -1759,7 +1755,7 @@
         <v>3.7300572839798822</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>2329.8085122481007</v>
@@ -1773,7 +1769,7 @@
         <v>2.9544157494105017</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>3028.7510659225309</v>
@@ -1787,7 +1783,7 @@
         <v>2.3142382660355136</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>3937.37638569929</v>
@@ -1801,7 +1797,7 @@
         <v>1.7999715595587391</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>5118.5893014090771</v>
@@ -1815,7 +1811,7 @@
         <v>1.3938430645516291</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>6654.1660918318003</v>
@@ -1829,7 +1825,7 @@
         <v>1.0764648052400858</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>8650.4159193813412</v>
@@ -1843,7 +1839,7 @@
         <v>0.83001562113666261</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>11245.540695195745</v>
@@ -1857,7 +1853,7 @@
         <v>0.63937339452175657</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>14619.202903754469</v>
@@ -1871,7 +1867,7 @@
         <v>0.49223664547294987</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>19004.963774880809</v>
@@ -1885,7 +1881,7 @@
         <v>0.37883100090695393</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>24706.452907345054</v>
@@ -1899,7 +1895,7 @@
         <v>0.29149387376123542</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>32118.388779548572</v>
@@ -1913,7 +1909,7 @@
         <v>0.22426496038931817</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>41753.905413413144</v>
@@ -1927,7 +1923,7 @@
         <v>0.17252922295281248</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>54280.077037437091</v>
@@ -1941,7 +1937,7 @@
         <v>0.13272285211432147</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>70564.100148668222</v>
@@ -1955,7 +1951,7 @@
         <v>0.10209817317754599</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>91733.330193268688</v>
@@ -1969,7 +1965,7 @@
         <v>7.8538727599663863E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>119253.32925124929</v>
@@ -1983,7 +1979,7 @@
         <v>6.0415166607917813E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>155029.32802662408</v>
@@ -1997,7 +1993,7 @@
         <v>4.6473551366534603E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="2"/>
         <v>201538.1264346113</v>
@@ -2011,7 +2007,7 @@
         <v>3.5749043285901221E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>261999.5643649947</v>
@@ -2025,7 +2021,7 @@
         <v>2.7499335809817227E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="2"/>
         <v>340599.43367449311</v>
@@ -2039,7 +2035,7 @@
         <v>2.1153367893844963E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="2"/>
         <v>442779.26377684105</v>
@@ -2053,7 +2049,7 @@
         <v>1.6271836320547274E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="2"/>
         <v>575613.04290989344</v>
@@ -2067,7 +2063,7 @@
         <v>1.2516803935139176E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="2"/>
         <v>748296.95578286145</v>
@@ -2081,7 +2077,7 @@
         <v>9.6283137987625694E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>972786.04251771991</v>
@@ -2095,7 +2091,7 @@
         <v>7.4063966314682926E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>1264621.8552730358</v>
@@ -2109,7 +2105,7 @@
         <v>5.6972288160368591E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>1644008.4118549465</v>
@@ -2123,7 +2119,7 @@
         <v>4.3824839950326747E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="2"/>
         <v>2137210.9354114304</v>
@@ -2137,7 +2133,7 @@
         <v>3.3711416668157513E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>2778374.2160348599</v>
@@ -2151,7 +2147,7 @@
         <v>2.5931859577122719E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>3611886.4808453182</v>
@@ -2165,7 +2161,7 @@
         <v>1.9947584563930077E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>4695452.4250989137</v>
@@ -2179,7 +2175,7 @@
         <v>1.5344295943048483E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>6104088.1526285885</v>
@@ -2193,7 +2189,7 @@
         <v>1.1803304628307996E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="2"/>
         <v>7935314.5984171657</v>
@@ -2207,7 +2203,7 @@
         <v>9.0794651245210524E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>10315908.977942316</v>
@@ -2221,7 +2217,7 @@
         <v>6.9842039536928413E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>13410681.671325011</v>
@@ -2235,7 +2231,7 @@
         <v>5.3724645851135531E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>17433886.172722515</v>
@@ -2249,7 +2245,7 @@
         <v>4.1326650679070236E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>22664052.02453927</v>
@@ -2263,7 +2259,7 @@
         <v>3.1789731302676058E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="2"/>
         <v>29463267.631901052</v>
@@ -2277,7 +2273,7 @@
         <v>2.4453639468641826E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>38302247.921471372</v>
@@ -2291,7 +2287,7 @@
         <v>1.8810491901251504E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>49792922.297912784</v>
@@ -2305,7 +2301,7 @@
         <v>1.4469609155854025E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>64730798.98728662</v>
@@ -2319,7 +2315,7 @@
         <v>1.1130468581901898E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>84150038.683472604</v>
@@ -2333,7 +2329,7 @@
         <v>8.5618989093718447E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>109395050.28851439</v>
@@ -2347,7 +2343,7 @@
         <v>6.5860760842307474E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>142213565.37506872</v>
@@ -2371,25 +2367,25 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2397,31 +2393,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>4.7E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.3000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>4.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.3000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2429,7 +2425,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -2443,7 +2439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2481,1006 +2477,1006 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
         <f t="shared" ref="B9:B28" si="0">-1/(2*PI()*A9*$D$3)</f>
-        <v>-338627.53849339433</v>
+        <v>-48228.770633907683</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C18" si="1">-1/(2*PI()*A9*$D$4)</f>
-        <v>-318309.88618379069</v>
+        <v>-48228.770633907683</v>
       </c>
       <c r="D9">
         <f>($D$1*B9^2)/($D$1^2+B9^2)</f>
-        <v>9.9999999912792177</v>
+        <v>9.9999995700800515</v>
       </c>
       <c r="E9">
         <f>(B9*D1^2+C9*($D$1^2+B9^2))/($D$1^2+B9^2)</f>
-        <v>-318309.88647910039</v>
+        <v>-48228.772707358745</v>
       </c>
       <c r="F9">
         <f>$D$5*(B9^2)/($D$1^2+B9^2)</f>
-        <v>99.999999912792177</v>
+        <v>99.999995700800511</v>
       </c>
       <c r="G9">
         <f>$D$5*($D$1*B9)/($D$1^2+B9^2)</f>
-        <v>-2.9530970917990736E-3</v>
+        <v>-2.0734510622274618E-2</v>
       </c>
       <c r="H9">
         <f>((D9+$D$2)*F9+E9*G9)/((D9+$D$2)^2+E9^2)</f>
-        <v>1.0060973405314726E-6</v>
+        <v>8.6693243091507771E-5</v>
       </c>
       <c r="I9">
         <f>((D9+$D$2)*G9-E9*F9)/((D9+$D$2)^2+E9^2)</f>
-        <v>3.1415607243805794E-4</v>
+        <v>2.0698379137272225E-3</v>
       </c>
       <c r="J9">
         <f>$D$2*H9</f>
-        <v>1.0060973405314727E-3</v>
+        <v>0.17338648618301555</v>
       </c>
       <c r="K9">
         <f>$D$2*I9</f>
-        <v>0.31415607243805793</v>
+        <v>4.139675827454445</v>
       </c>
       <c r="L9">
         <f>SQRT(J9^2+K9^2)</f>
-        <v>0.31415768346733924</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.1433053025334177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>A9*2</f>
         <v>2</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>-169313.76924669716</v>
+        <v>-24114.385316953842</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-159154.94309189534</v>
+        <v>-24114.385316953842</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:D18" si="2">($D$1*B10^2)/($D$1^2+B10^2)</f>
-        <v>9.9999999651168707</v>
+        <v>9.9999982803204244</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:E18" si="3">(B10+C10*($D$1^2+B10^2))/($D$1^2+B10^2)</f>
-        <v>-159154.94309780156</v>
+        <v>-24114.385358422856</v>
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F18" si="4">$D$5*(B10^2)/($D$1^2+B10^2)</f>
-        <v>99.999999651168693</v>
+        <v>99.999982803204247</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G18" si="5">$D$5*($D$1*B10)/($D$1^2+B10^2)</f>
-        <v>-5.9061941681461567E-3</v>
+        <v>-4.1469015896042079E-2</v>
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H18" si="6">((D10+$D$2)*F10+E10*G10)/((D10+$D$2)^2+E10^2)</f>
-        <v>4.0242678110678465E-6</v>
+        <v>3.4497847312710538E-4</v>
       </c>
       <c r="I10">
         <f t="shared" ref="I10:I18" si="7">((D10+$D$2)*G10-E10*F10)/((D10+$D$2)^2+E10^2)</f>
-        <v>6.2829299043028544E-4</v>
+        <v>4.1181466828523351E-3</v>
       </c>
       <c r="J10">
         <f t="shared" ref="J10:J18" si="8">$D$2*H10</f>
-        <v>4.0242678110678463E-3</v>
+        <v>0.68995694625421078</v>
       </c>
       <c r="K10">
         <f t="shared" ref="K10:K18" si="9">$D$2*I10</f>
-        <v>0.62829299043028541</v>
+        <v>8.23629336570467</v>
       </c>
       <c r="L10">
         <f t="shared" ref="L10:L18" si="10">SQRT(J10^2+K10^2)</f>
-        <v>0.62830587817976513</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.2651418011813451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" ref="A11:A18" si="11">A10*2</f>
         <v>4</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>-84656.884623348582</v>
+        <v>-12057.192658476921</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>-79577.471545947672</v>
+        <v>-12057.192658476921</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>9.9999998604674829</v>
+        <v>9.9999931212852484</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>-79577.471557760058</v>
+        <v>-12057.19274141491</v>
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>99.999998604674815</v>
+        <v>99.999931212852488</v>
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>-1.1812388212676394E-2</v>
+        <v>-8.2937989004054441E-2</v>
       </c>
       <c r="H11">
         <f t="shared" si="6"/>
-        <v>1.6095126603286144E-5</v>
+        <v>1.3519292761660212E-3</v>
       </c>
       <c r="I11">
         <f t="shared" si="7"/>
-        <v>1.2564327638160272E-3</v>
+        <v>8.0684248368117426E-3</v>
       </c>
       <c r="J11">
         <f t="shared" si="8"/>
-        <v>1.6095126603286145E-2</v>
+        <v>2.7038585523320426</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>1.2564327638160271</v>
+        <v>16.136849673623484</v>
       </c>
       <c r="L11">
         <f t="shared" si="10"/>
-        <v>1.2565358503006416</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>16.361808227092183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>-42328.442311674291</v>
+        <v>-6028.5963292384604</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>-39788.735772973836</v>
+        <v>-6028.5963292384604</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>9.9999994418699547</v>
+        <v>9.9999724851977732</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>-39788.735796598616</v>
+        <v>-6028.5964951140959</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>99.999994418699544</v>
+        <v>99.999724851977732</v>
       </c>
       <c r="G12">
         <f t="shared" si="5"/>
-        <v>-2.3624775436425473E-2</v>
+        <v>-0.16587563570475422</v>
       </c>
       <c r="H12">
         <f t="shared" si="6"/>
-        <v>6.4349410940813174E-5</v>
+        <v>5.0019577896588969E-3</v>
       </c>
       <c r="I12">
         <f t="shared" si="7"/>
-        <v>2.5116405312437273E-3</v>
+        <v>1.4919855708586269E-2</v>
       </c>
       <c r="J12">
         <f t="shared" si="8"/>
-        <v>6.4349410940813173E-2</v>
+        <v>10.003915579317793</v>
       </c>
       <c r="K12">
         <f t="shared" si="9"/>
-        <v>2.5116405312437271</v>
+        <v>29.839711417172538</v>
       </c>
       <c r="L12">
         <f t="shared" si="10"/>
-        <v>2.5124647270906517</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>31.47199873503833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>-21164.221155837145</v>
+        <v>-3014.2981646192302</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>-19894.367886486918</v>
+        <v>-3014.2981646192302</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>9.9999977674801919</v>
+        <v>9.9998899416995624</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>-19894.367933736459</v>
+        <v>-3014.2984963677632</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>99.999977674801912</v>
+        <v>99.998899416995627</v>
       </c>
       <c r="G13">
         <f t="shared" si="5"/>
-        <v>-4.724954296143407E-2</v>
+        <v>-0.33174853301092594</v>
       </c>
       <c r="H13">
         <f t="shared" si="6"/>
-        <v>2.5690131530347877E-4</v>
+        <v>1.538902211143702E-2</v>
       </c>
       <c r="I13">
         <f t="shared" si="7"/>
-        <v>5.01350471043521E-3</v>
+        <v>2.2913114527284773E-2</v>
       </c>
       <c r="J13">
         <f t="shared" si="8"/>
-        <v>0.25690131530347876</v>
+        <v>30.778044222874041</v>
       </c>
       <c r="K13">
         <f t="shared" si="9"/>
-        <v>5.0135047104352104</v>
+        <v>45.826229054569545</v>
       </c>
       <c r="L13">
         <f t="shared" si="10"/>
-        <v>5.0200824462712461</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>55.20263830241327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>-10582.110577918573</v>
+        <v>-1507.1490823096151</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>-9947.183943243459</v>
+        <v>-1507.1490823096151</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>9.9999910699267467</v>
+        <v>9.9995597813331649</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>-9947.1840377424815</v>
+        <v>-1507.1497457847747</v>
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
-        <v>99.99991069926746</v>
+        <v>99.995597813331642</v>
       </c>
       <c r="G14">
         <f t="shared" si="5"/>
-        <v>-9.4499022631586174E-2</v>
+        <v>-0.66347515973731286</v>
       </c>
       <c r="H14">
         <f t="shared" si="6"/>
-        <v>1.0197399772232999E-3</v>
+        <v>3.2003154388486374E-2</v>
       </c>
       <c r="I14">
         <f t="shared" si="7"/>
-        <v>9.9495468220812747E-3</v>
+        <v>2.366670709438163E-2</v>
       </c>
       <c r="J14">
         <f t="shared" si="8"/>
-        <v>1.0197399772232998</v>
+        <v>64.006308776972745</v>
       </c>
       <c r="K14">
         <f t="shared" si="9"/>
-        <v>9.9495468220812739</v>
+        <v>47.333414188763257</v>
       </c>
       <c r="L14">
         <f t="shared" si="10"/>
-        <v>10.001667440278894</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79.606907125061667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>-5291.0552889592864</v>
+        <v>-753.57454115480755</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>-4973.5919716217295</v>
+        <v>-753.57454115480755</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>9.9999642798026844</v>
+        <v>9.9982393578529187</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>-4973.5921606192687</v>
+        <v>-753.5758679299056</v>
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>99.999642798026827</v>
+        <v>99.982393578529184</v>
       </c>
       <c r="G15">
         <f t="shared" si="5"/>
-        <v>-0.18899753893461216</v>
+        <v>-1.3267750981251594</v>
       </c>
       <c r="H15">
         <f t="shared" si="6"/>
-        <v>3.9577879735405866E-3</v>
+        <v>4.3829339642092312E-2</v>
       </c>
       <c r="I15">
         <f t="shared" si="7"/>
-        <v>1.9302402365490787E-2</v>
+        <v>1.5772132006238573E-2</v>
       </c>
       <c r="J15">
         <f t="shared" si="8"/>
-        <v>3.9577879735405865</v>
+        <v>87.658679284184629</v>
       </c>
       <c r="K15">
         <f t="shared" si="9"/>
-        <v>19.302402365490785</v>
+        <v>31.544264012477147</v>
       </c>
       <c r="L15">
         <f t="shared" si="10"/>
-        <v>19.703979870138081</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>93.161604998713926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>-2645.5276444796432</v>
+        <v>-376.78727057740377</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>-2486.7959858108647</v>
+        <v>-376.78727057740377</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>9.9998571207418365</v>
+        <v>9.9929611492808448</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>-2486.7963638018923</v>
+        <v>-376.78992272675424</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>99.998571207418351</v>
+        <v>99.929611492808448</v>
       </c>
       <c r="G16">
         <f t="shared" si="5"/>
-        <v>-0.37799102729500061</v>
+        <v>-2.6521493504722797</v>
       </c>
       <c r="H16">
         <f t="shared" si="6"/>
-        <v>1.4149765254645983E-2</v>
+        <v>4.8267593194601048E-2</v>
       </c>
       <c r="I16">
         <f t="shared" si="7"/>
-        <v>3.4464949189044913E-2</v>
+        <v>7.7286804778885576E-3</v>
       </c>
       <c r="J16">
         <f t="shared" si="8"/>
-        <v>14.149765254645983</v>
+        <v>96.535186389202096</v>
       </c>
       <c r="K16">
         <f t="shared" si="9"/>
-        <v>34.464949189044916</v>
+        <v>15.457360955777116</v>
       </c>
       <c r="L16">
         <f t="shared" si="10"/>
-        <v>37.256523983928432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97.764882339801204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="11"/>
         <v>256</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>-1322.7638222398216</v>
+        <v>-188.39363528870189</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>-1243.3979929054324</v>
+        <v>-188.39363528870189</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>9.9994285074636746</v>
+        <v>9.9719039263438578</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>-1243.398748855084</v>
+        <v>-188.39892841015532</v>
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
-        <v>99.994285074636736</v>
+        <v>99.719039263438574</v>
       </c>
       <c r="G17">
         <f t="shared" si="5"/>
-        <v>-0.75594965173236672</v>
+        <v>-5.2931214534198654</v>
       </c>
       <c r="H17">
         <f t="shared" si="6"/>
-        <v>3.9722753109844154E-2</v>
+        <v>4.9424761199254576E-2</v>
       </c>
       <c r="I17">
         <f t="shared" si="7"/>
-        <v>4.8153761767963071E-2</v>
+        <v>1.9992570968767024E-3</v>
       </c>
       <c r="J17">
         <f t="shared" si="8"/>
-        <v>39.722753109844156</v>
+        <v>98.849522398509151</v>
       </c>
       <c r="K17">
         <f t="shared" si="9"/>
-        <v>48.153761767963069</v>
+        <v>3.9985141937534046</v>
       </c>
       <c r="L17">
         <f t="shared" si="10"/>
-        <v>62.423408165778447</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>98.930360325690771</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="11"/>
         <v>512</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>-661.3819111199108</v>
+        <v>-94.196817644350944</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>-621.69899645271619</v>
+        <v>-94.196817644350944</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>9.9977144217119758</v>
+        <v>9.8885550549905066</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>-621.70050809285237</v>
+        <v>-94.207315403513391</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>99.977144217119744</v>
+        <v>98.885550549905062</v>
       </c>
       <c r="G18">
         <f t="shared" si="5"/>
-        <v>-1.5116401361481073</v>
+        <v>-10.497759162443987</v>
       </c>
       <c r="H18">
         <f t="shared" si="6"/>
-        <v>7.2455548340738252E-2</v>
+        <v>4.9335943895842588E-2</v>
       </c>
       <c r="I18">
         <f t="shared" si="7"/>
-        <v>4.3103078808808079E-2</v>
+        <v>-2.9105854254482533E-3</v>
       </c>
       <c r="J18">
         <f t="shared" si="8"/>
-        <v>72.455548340738247</v>
+        <v>98.67188779168518</v>
       </c>
       <c r="K18">
         <f t="shared" si="9"/>
-        <v>43.103078808808078</v>
+        <v>-5.8211708508965065</v>
       </c>
       <c r="L18">
         <f t="shared" si="10"/>
-        <v>84.307069028376134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>98.843449304697174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" ref="A19:A28" si="12">A18*2</f>
         <v>1024</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>-330.6909555599554</v>
+        <v>-47.098408822175472</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:C28" si="13">-1/(2*PI()*A19*$D$4)</f>
-        <v>-310.84949822635809</v>
+        <v>-47.098408822175472</v>
       </c>
       <c r="D19">
         <f t="shared" ref="D19:D28" si="14">($D$1*B19^2)/($D$1^2+B19^2)</f>
-        <v>9.9908639511943367</v>
+        <v>9.5686420198743782</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:E28" si="15">(B19+C19*($D$1^2+B19^2))/($D$1^2+B19^2)</f>
-        <v>-310.85251943506768</v>
+        <v>-47.118725096672136</v>
       </c>
       <c r="F19">
         <f t="shared" ref="F19:F28" si="16">$D$5*(B19^2)/($D$1^2+B19^2)</f>
-        <v>99.908639511943363</v>
+        <v>95.686420198743775</v>
       </c>
       <c r="G19">
         <f t="shared" ref="G19:G28" si="17">$D$5*($D$1*B19)/($D$1^2+B19^2)</f>
-        <v>-3.0212087095871474</v>
+        <v>-20.316274496664413</v>
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H28" si="18">((D19+$D$2)*F19+E19*G19)/((D19+$D$2)^2+E19^2)</f>
-        <v>9.1201733130570353E-2</v>
+        <v>4.7826154930045064E-2</v>
       </c>
       <c r="I19">
         <f t="shared" ref="I19:I28" si="19">((D19+$D$2)*G19-E19*F19)/((D19+$D$2)^2+E19^2)</f>
-        <v>2.5078523692585897E-2</v>
+        <v>-8.9883802286690566E-3</v>
       </c>
       <c r="J19">
         <f t="shared" ref="J19:J28" si="20">$D$2*H19</f>
-        <v>91.201733130570346</v>
+        <v>95.652309860090128</v>
       </c>
       <c r="K19">
         <f t="shared" ref="K19:K28" si="21">$D$2*I19</f>
-        <v>25.078523692585897</v>
+        <v>-17.976760457338113</v>
       </c>
       <c r="L19">
         <f t="shared" ref="L19:L28" si="22">SQRT(J19^2+K19^2)</f>
-        <v>94.586936077977313</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97.326914561755274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="12"/>
         <v>2048</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>-165.3454777799777</v>
+        <v>-23.549204411087736</v>
       </c>
       <c r="C20">
         <f t="shared" si="13"/>
-        <v>-155.42474911317905</v>
+        <v>-23.549204411087736</v>
       </c>
       <c r="D20">
         <f t="shared" si="14"/>
-        <v>9.9635556918706758</v>
+        <v>8.4722679082753416</v>
       </c>
       <c r="E20">
         <f t="shared" si="15"/>
-        <v>-155.43077501471905</v>
+        <v>-23.585181286401138</v>
       </c>
       <c r="F20">
         <f t="shared" si="16"/>
-        <v>99.63555691870674</v>
+        <v>84.722679082753416</v>
       </c>
       <c r="G20">
         <f t="shared" si="17"/>
-        <v>-6.0259015400040159</v>
+        <v>-35.976875313402608</v>
       </c>
       <c r="H20">
         <f t="shared" si="18"/>
-        <v>9.7267132950951865E-2</v>
+        <v>4.2387147653844978E-2</v>
       </c>
       <c r="I20">
         <f t="shared" si="19"/>
-        <v>9.0027053617726255E-3</v>
+        <v>-1.7414811899892555E-2</v>
       </c>
       <c r="J20">
         <f t="shared" si="20"/>
-        <v>97.267132950951861</v>
+        <v>84.774295307689954</v>
       </c>
       <c r="K20">
         <f t="shared" si="21"/>
-        <v>9.0027053617726249</v>
+        <v>-34.829623799785111</v>
       </c>
       <c r="L20">
         <f t="shared" si="22"/>
-        <v>97.682873915180423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91.650334636322967</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="12"/>
         <v>4096</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>-82.67273888998885</v>
+        <v>-11.774602205543868</v>
       </c>
       <c r="C21">
         <f t="shared" si="13"/>
-        <v>-77.712374556589523</v>
+        <v>-11.774602205543868</v>
       </c>
       <c r="D21">
         <f t="shared" si="14"/>
-        <v>9.8557993553010554</v>
+        <v>5.8096097374059861</v>
       </c>
       <c r="E21">
         <f t="shared" si="15"/>
-        <v>-77.724296018836483</v>
+        <v>-11.823942383971897</v>
       </c>
       <c r="F21">
         <f t="shared" si="16"/>
-        <v>98.557993553010547</v>
+        <v>58.096097374059859</v>
       </c>
       <c r="G21">
         <f t="shared" si="17"/>
-        <v>-11.921462246963891</v>
+        <v>-49.340178428029027</v>
       </c>
       <c r="H21">
         <f t="shared" si="18"/>
-        <v>9.7924616701361059E-2</v>
+        <v>2.91079079002525E-2</v>
       </c>
       <c r="I21">
         <f t="shared" si="19"/>
-        <v>-4.268273107594131E-3</v>
+        <v>-2.442704829224189E-2</v>
       </c>
       <c r="J21">
         <f t="shared" si="20"/>
-        <v>97.92461670136106</v>
+        <v>58.215815800504998</v>
       </c>
       <c r="K21">
         <f t="shared" si="21"/>
-        <v>-4.2682731075941307</v>
+        <v>-48.854096584483777</v>
       </c>
       <c r="L21">
         <f t="shared" si="22"/>
-        <v>98.01759388716647</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>75.998710268032823</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="12"/>
         <v>8192</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>-41.336369444994425</v>
+        <v>-5.887301102771934</v>
       </c>
       <c r="C22">
         <f t="shared" si="13"/>
-        <v>-38.856187278294762</v>
+        <v>-5.887301102771934</v>
       </c>
       <c r="D22">
         <f t="shared" si="14"/>
-        <v>9.4471153194193906</v>
+        <v>2.5739071278264283</v>
       </c>
       <c r="E22">
         <f t="shared" si="15"/>
-        <v>-38.87904152371172</v>
+        <v>-5.931020747527568</v>
       </c>
       <c r="F22">
         <f t="shared" si="16"/>
-        <v>94.471153194193903</v>
+        <v>25.739071278264284</v>
       </c>
       <c r="G22">
         <f t="shared" si="17"/>
-        <v>-22.854245416957816</v>
+        <v>-43.71964475563427</v>
       </c>
       <c r="H22">
         <f t="shared" si="18"/>
-        <v>9.4319108581619016E-2</v>
+        <v>1.291754012055938E-2</v>
       </c>
       <c r="I22">
         <f t="shared" si="19"/>
-        <v>-1.9007641496763473E-2</v>
+        <v>-2.1793468097148452E-2</v>
       </c>
       <c r="J22">
         <f t="shared" si="20"/>
-        <v>94.31910858161902</v>
+        <v>25.83508024111876</v>
       </c>
       <c r="K22">
         <f t="shared" si="21"/>
-        <v>-19.007641496763473</v>
+        <v>-43.586936194296904</v>
       </c>
       <c r="L22">
         <f t="shared" si="22"/>
-        <v>96.215303766608372</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50.668258089959579</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="12"/>
         <v>16384</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>-20.668184722497212</v>
+        <v>-2.943650551385967</v>
       </c>
       <c r="C23">
         <f t="shared" si="13"/>
-        <v>-19.428093639147381</v>
+        <v>-2.943650551385967</v>
       </c>
       <c r="D23">
         <f t="shared" si="14"/>
-        <v>8.1030925916453125</v>
+        <v>0.79741152197287468</v>
       </c>
       <c r="E23">
         <f t="shared" si="15"/>
-        <v>-19.467299271864729</v>
+        <v>-2.9707397560334896</v>
       </c>
       <c r="F23">
         <f t="shared" si="16"/>
-        <v>81.030925916453114</v>
+        <v>7.9741152197287475</v>
       </c>
       <c r="G23">
         <f t="shared" si="17"/>
-        <v>-39.205632717348117</v>
+        <v>-27.089204647522692</v>
       </c>
       <c r="H23">
         <f t="shared" si="18"/>
-        <v>8.1100367098855417E-2</v>
+        <v>4.0055624610291687E-3</v>
       </c>
       <c r="I23">
         <f t="shared" si="19"/>
-        <v>-3.7324384655189419E-2</v>
+        <v>-1.3533256794488349E-2</v>
       </c>
       <c r="J23">
         <f t="shared" si="20"/>
-        <v>81.100367098855415</v>
+        <v>8.0111249220583378</v>
       </c>
       <c r="K23">
         <f t="shared" si="21"/>
-        <v>-37.324384655189419</v>
+        <v>-27.066513588976697</v>
       </c>
       <c r="L23">
         <f t="shared" si="22"/>
-        <v>89.276980423049977</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28.227190444305368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="12"/>
         <v>32768</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>-10.334092361248606</v>
+        <v>-1.4718252756929835</v>
       </c>
       <c r="C24">
         <f t="shared" si="13"/>
-        <v>-9.7140468195736904</v>
+        <v>-1.4718252756929835</v>
       </c>
       <c r="D24">
         <f t="shared" si="14"/>
-        <v>5.1642572441321963</v>
+        <v>0.2120337416405588</v>
       </c>
       <c r="E24">
         <f t="shared" si="15"/>
-        <v>-9.7640198318480671</v>
+        <v>-1.4862314518296671</v>
       </c>
       <c r="F24">
         <f t="shared" si="16"/>
-        <v>51.64257244132196</v>
+        <v>2.1203374164055879</v>
       </c>
       <c r="G24">
         <f t="shared" si="17"/>
-        <v>-49.97301227437675</v>
+        <v>-14.406176136683504</v>
       </c>
       <c r="H24">
         <f t="shared" si="18"/>
-        <v>5.1855290694105237E-2</v>
+        <v>1.0654073293730856E-3</v>
       </c>
       <c r="I24">
         <f t="shared" si="19"/>
-        <v>-4.9212549920225515E-2</v>
+        <v>-7.2015328634214993E-3</v>
       </c>
       <c r="J24">
         <f t="shared" si="20"/>
-        <v>51.855290694105236</v>
+        <v>2.1308146587461714</v>
       </c>
       <c r="K24">
         <f t="shared" si="21"/>
-        <v>-49.212549920225513</v>
+        <v>-14.403065726842998</v>
       </c>
       <c r="L24">
         <f t="shared" si="22"/>
-        <v>71.490182840868755</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>14.55983081775633</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="12"/>
         <v>65536</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>-5.1670461806243031</v>
+        <v>-0.73591263784649175</v>
       </c>
       <c r="C25">
         <f t="shared" si="13"/>
-        <v>-4.8570234097868452</v>
+        <v>-0.73591263784649175</v>
       </c>
       <c r="D25">
         <f t="shared" si="14"/>
-        <v>2.1072383982969343</v>
+        <v>5.3865025629727371E-2</v>
       </c>
       <c r="E25">
         <f t="shared" si="15"/>
-        <v>-4.8978056734755038</v>
+        <v>-0.74323212427185792</v>
       </c>
       <c r="F25">
         <f t="shared" si="16"/>
-        <v>21.072383982969342</v>
+        <v>0.5386502562972737</v>
       </c>
       <c r="G25">
         <f t="shared" si="17"/>
-        <v>-40.782263688657977</v>
+        <v>-7.3194864253660752</v>
       </c>
       <c r="H25">
         <f t="shared" si="18"/>
-        <v>2.1226470209594551E-2</v>
+        <v>2.7067778346994992E-4</v>
       </c>
       <c r="I25">
         <f t="shared" si="19"/>
-        <v>-4.0592761935793545E-2</v>
+        <v>-3.6595440637536437E-3</v>
       </c>
       <c r="J25">
         <f t="shared" si="20"/>
-        <v>21.226470209594552</v>
+        <v>0.54135556693989983</v>
       </c>
       <c r="K25">
         <f t="shared" si="21"/>
-        <v>-40.592761935793547</v>
+        <v>-7.3190881275072872</v>
       </c>
       <c r="L25">
         <f t="shared" si="22"/>
-        <v>45.807590627916838</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3390814730506264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="12"/>
         <v>131072</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>-2.5835230903121515</v>
+        <v>-0.36795631892324587</v>
       </c>
       <c r="C26">
         <f t="shared" si="13"/>
-        <v>-2.4285117048934226</v>
+        <v>-0.36795631892324587</v>
       </c>
       <c r="D26">
         <f t="shared" si="14"/>
-        <v>0.62569647192283795</v>
+        <v>1.3520879094855406E-2</v>
       </c>
       <c r="E26">
         <f t="shared" si="15"/>
-        <v>-2.4527304345138048</v>
+        <v>-0.37163090701957802</v>
       </c>
       <c r="F26">
         <f t="shared" si="16"/>
-        <v>6.2569647192283782</v>
+        <v>0.13520879094855406</v>
       </c>
       <c r="G26">
         <f t="shared" si="17"/>
-        <v>-24.218729620382014</v>
+        <v>-3.6745880963321094</v>
       </c>
       <c r="H26">
         <f t="shared" si="18"/>
-        <v>6.3123420293378042E-3</v>
+        <v>6.7945329106836944E-5</v>
       </c>
       <c r="I26">
         <f t="shared" si="19"/>
-        <v>-2.4188112730175855E-2</v>
+        <v>-1.8372690021278915E-3</v>
       </c>
       <c r="J26">
         <f t="shared" si="20"/>
-        <v>6.3123420293378043</v>
+        <v>0.13589065821367388</v>
       </c>
       <c r="K26">
         <f t="shared" si="21"/>
-        <v>-24.188112730175856</v>
+        <v>-3.6745380042557829</v>
       </c>
       <c r="L26">
         <f t="shared" si="22"/>
-        <v>24.99820912271597</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.6770498794155375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="12"/>
         <v>262144</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>-1.2917615451560758</v>
+        <v>-0.18397815946162294</v>
       </c>
       <c r="C27">
         <f t="shared" si="13"/>
-        <v>-1.2142558524467113</v>
+        <v>-0.18397815946162294</v>
       </c>
       <c r="D27">
         <f t="shared" si="14"/>
-        <v>0.16412610221362278</v>
+        <v>3.3836510189383202E-3</v>
       </c>
       <c r="E27">
         <f t="shared" si="15"/>
-        <v>-1.2269614561108761</v>
+        <v>-0.18581731853835246</v>
       </c>
       <c r="F27">
         <f t="shared" si="16"/>
-        <v>1.6412610221362276</v>
+        <v>3.3836510189383204E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="17"/>
-        <v>-12.705603664164842</v>
+        <v>-1.8391590767295045</v>
       </c>
       <c r="H27">
         <f t="shared" si="18"/>
-        <v>1.6565733695364084E-3</v>
+        <v>1.7003662938141946E-5</v>
       </c>
       <c r="I27">
         <f t="shared" si="19"/>
-        <v>-1.270148646702505E-2</v>
+        <v>-9.1957640281440994E-4</v>
       </c>
       <c r="J27">
         <f t="shared" si="20"/>
-        <v>1.6565733695364084</v>
+        <v>3.4007325876283891E-2</v>
       </c>
       <c r="K27">
         <f t="shared" si="21"/>
-        <v>-12.701486467025051</v>
+        <v>-1.8391528056288198</v>
       </c>
       <c r="L27">
         <f t="shared" si="22"/>
-        <v>12.809059052119235</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8394671893419614</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="12"/>
         <v>524288</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>-0.64588077257803789</v>
+        <v>-9.1989079730811468E-2</v>
       </c>
       <c r="C28">
         <f t="shared" si="13"/>
-        <v>-0.60712792622335565</v>
+        <v>-9.1989079730811468E-2</v>
       </c>
       <c r="D28">
         <f t="shared" si="14"/>
-        <v>4.1542896073951951E-2</v>
+        <v>8.4612747974275378E-4</v>
       </c>
       <c r="E28">
         <f t="shared" si="15"/>
-        <v>-0.61355990219132472</v>
+        <v>-9.2908892693631395E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="16"/>
-        <v>0.41542896073951946</v>
+        <v>8.4612747974275385E-3</v>
       </c>
       <c r="G28">
         <f t="shared" si="17"/>
-        <v>-6.4319759679690058</v>
+        <v>-0.9198129628199182</v>
       </c>
       <c r="H28">
         <f t="shared" si="18"/>
-        <v>4.1935762015408046E-4</v>
+        <v>4.2520002825973336E-6</v>
       </c>
       <c r="I28">
         <f t="shared" si="19"/>
-        <v>-6.4314514858279208E-3</v>
+        <v>-4.5990608931605E-4</v>
       </c>
       <c r="J28">
         <f t="shared" si="20"/>
-        <v>0.41935762015408046</v>
+        <v>8.5040005651946665E-3</v>
       </c>
       <c r="K28">
         <f t="shared" si="21"/>
-        <v>-6.431451485827921</v>
+        <v>-0.91981217863209996</v>
       </c>
       <c r="L28">
         <f t="shared" si="22"/>
-        <v>6.4451089229073135</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>0.9198514890924202</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>20</v>
       </c>
@@ -3492,18 +3488,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3645,14 +3641,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{661D9C9A-FCC2-478F-B8DB-C85B278F20B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F441C0-5076-47A9-8E1B-B9BDAE937C6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3664,6 +3652,14 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{661D9C9A-FCC2-478F-B8DB-C85B278F20B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>